<commit_message>
Made changes to statistical models
</commit_message>
<xml_diff>
--- a/analysis/s0_model_summary.xlsx
+++ b/analysis/s0_model_summary.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -421,13 +421,13 @@
         </is>
       </c>
       <c r="B2">
-        <v>-3.581785597488453</v>
+        <v>-3.403294699040295</v>
       </c>
       <c r="C2">
-        <v>0.01226987670351449</v>
+        <v>0.007025203729177106</v>
       </c>
       <c r="D2">
-        <v>-291.9169999860321</v>
+        <v>-484.4407123605138</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -438,29 +438,29 @@
         </is>
       </c>
       <c r="I2">
-        <v>0.02782596789087361</v>
+        <v>0.03326349601517221</v>
       </c>
       <c r="J2">
-        <v>0.02716476483772319</v>
+        <v>0.03280861655154064</v>
       </c>
       <c r="K2">
-        <v>0.02850326493490182</v>
+        <v>0.03372468221612411</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>I(o_htn &gt;= 1)TRUE</t>
+          <t>I(o_htn_blood_related &gt;= 1)TRUE</t>
         </is>
       </c>
       <c r="B3">
-        <v>0.5923664131619305</v>
+        <v>0.5063385776687654</v>
       </c>
       <c r="C3">
-        <v>0.006825841372258525</v>
+        <v>0.004284181332685049</v>
       </c>
       <c r="D3">
-        <v>86.7829152270395</v>
+        <v>118.1879426544779</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -471,32 +471,32 @@
         </is>
       </c>
       <c r="I3">
-        <v>1.808262452402217</v>
+        <v>1.659205009423783</v>
       </c>
       <c r="J3">
-        <v>1.784231453180319</v>
+        <v>1.645331004072328</v>
       </c>
       <c r="K3">
-        <v>1.832617114186263</v>
+        <v>1.673196005231272</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>blood_relation1</t>
+          <t>age</t>
         </is>
       </c>
       <c r="B4">
-        <v>0.3237905710164796</v>
+        <v>0.04885590638950511</v>
       </c>
       <c r="C4">
-        <v>0.01467689914527649</v>
+        <v>0.0001324142441275275</v>
       </c>
       <c r="D4">
-        <v>22.06123839998492</v>
+        <v>368.9626196291406</v>
       </c>
       <c r="E4">
-        <v>7.451478414449636E-108</v>
+        <v>0</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -504,29 +504,29 @@
         </is>
       </c>
       <c r="I4">
-        <v>1.382357771019066</v>
+        <v>1.050069031600197</v>
       </c>
       <c r="J4">
-        <v>1.343158390874731</v>
+        <v>1.049796540531474</v>
       </c>
       <c r="K4">
-        <v>1.422701164716933</v>
+        <v>1.050341593398229</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>age</t>
+          <t>sexMale</t>
         </is>
       </c>
       <c r="B5">
-        <v>0.05186615670622972</v>
+        <v>0.1988034035354678</v>
       </c>
       <c r="C5">
-        <v>0.000260949611072481</v>
+        <v>0.004159194735318086</v>
       </c>
       <c r="D5">
-        <v>198.7592795906619</v>
+        <v>47.79853221281398</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -537,90 +537,80 @@
         </is>
       </c>
       <c r="I5">
-        <v>1.053234764669089</v>
+        <v>1.219942106017866</v>
       </c>
       <c r="J5">
-        <v>1.052696213648486</v>
+        <v>1.210037537499415</v>
       </c>
       <c r="K5">
-        <v>1.053773591208116</v>
+        <v>1.229927746796057</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>I(o_htn &gt;= 1)TRUE:blood_relation1</t>
-        </is>
-      </c>
       <c r="B6">
-        <v>-0.07829067662004638</v>
+        <v>-2.894066065584643</v>
       </c>
       <c r="C6">
-        <v>0.008570596853723137</v>
+        <v>0.004258553308631226</v>
       </c>
       <c r="D6">
-        <v>-9.134798655946145</v>
+        <v>-679.589019049957</v>
       </c>
       <c r="E6">
-        <v>6.55285980490217E-20</v>
+        <v>0</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="I6">
-        <v>0.9246956000830447</v>
+        <v>0.05535069488170349</v>
       </c>
       <c r="J6">
-        <v>0.9092919616388754</v>
+        <v>0.05489061841347789</v>
       </c>
       <c r="K6">
-        <v>0.9403601801029992</v>
+        <v>0.0558146275709507</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>blood_relation1:age</t>
-        </is>
-      </c>
       <c r="B7">
-        <v>-0.005217623519052598</v>
+        <v>0.3157457385270618</v>
       </c>
       <c r="C7">
-        <v>0.0003024388048677717</v>
+        <v>0.002746954979160104</v>
       </c>
       <c r="D7">
-        <v>-17.25183222217063</v>
+        <v>114.943907316458</v>
       </c>
       <c r="E7">
-        <v>1.084063804463716E-66</v>
+        <v>0</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="I7">
-        <v>0.9947959646356436</v>
+        <v>1.371281547230354</v>
       </c>
       <c r="J7">
-        <v>0.9942064441717353</v>
+        <v>1.363918363423921</v>
       </c>
       <c r="K7">
-        <v>0.9953858346591221</v>
+        <v>1.378684481565281</v>
       </c>
     </row>
     <row r="8">
       <c r="B8">
-        <v>-3.05107991496634</v>
+        <v>0.03085560690459519</v>
       </c>
       <c r="C8">
-        <v>0.007627025521219438</v>
+        <v>7.027810067695005E-05</v>
       </c>
       <c r="D8">
-        <v>-400.0353619478281</v>
+        <v>439.0500967923181</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -631,24 +621,24 @@
         </is>
       </c>
       <c r="I8">
-        <v>0.04730780838533869</v>
+        <v>1.031336575254143</v>
       </c>
       <c r="J8">
-        <v>0.04660586511246032</v>
+        <v>1.031194523501524</v>
       </c>
       <c r="K8">
-        <v>0.04802032381168209</v>
+        <v>1.031478646575039</v>
       </c>
     </row>
     <row r="9">
       <c r="B9">
-        <v>0.4106041183674009</v>
+        <v>0.132323953866347</v>
       </c>
       <c r="C9">
-        <v>0.004875937921551556</v>
+        <v>0.002741871625053018</v>
       </c>
       <c r="D9">
-        <v>84.21028425167971</v>
+        <v>48.26044832196998</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -659,125 +649,145 @@
         </is>
       </c>
       <c r="I9">
-        <v>1.507728356431902</v>
+        <v>1.141478045603087</v>
       </c>
       <c r="J9">
-        <v>1.493387874270988</v>
+        <v>1.135360118329808</v>
       </c>
       <c r="K9">
-        <v>1.522206545234307</v>
+        <v>1.147628939539116</v>
       </c>
     </row>
     <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>(Intercept)</t>
+        </is>
+      </c>
       <c r="B10">
-        <v>0.2641112639290071</v>
+        <v>-2.921883347998571</v>
       </c>
       <c r="C10">
-        <v>0.009074302127735152</v>
+        <v>0.008059633476183818</v>
       </c>
       <c r="D10">
-        <v>29.10540780009563</v>
+        <v>-362.5330303955786</v>
       </c>
       <c r="E10">
-        <v>3.066550601404892E-186</v>
+        <v>0</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="I10">
-        <v>1.302273084260338</v>
+        <v>0.05383220698968923</v>
       </c>
       <c r="J10">
-        <v>1.279316091671088</v>
+        <v>0.05298850744456744</v>
       </c>
       <c r="K10">
-        <v>1.325642034075933</v>
+        <v>0.05468934018215774</v>
       </c>
     </row>
     <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>I(o_htn_blood_related &gt;= 1)TRUE</t>
+        </is>
+      </c>
       <c r="B11">
-        <v>0.03334385515536203</v>
+        <v>0.3037747503343061</v>
       </c>
       <c r="C11">
-        <v>0.0001439509798338398</v>
+        <v>0.005536744292336373</v>
       </c>
       <c r="D11">
-        <v>231.6334018278325</v>
+        <v>54.86523023192036</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="I11">
-        <v>1.033905992031186</v>
+        <v>1.354963816566703</v>
       </c>
       <c r="J11">
-        <v>1.033614322889465</v>
+        <v>1.340339220457915</v>
       </c>
       <c r="K11">
-        <v>1.034197743477192</v>
+        <v>1.369747983333486</v>
       </c>
     </row>
     <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>age</t>
+        </is>
+      </c>
       <c r="B12">
-        <v>-0.09890708990173193</v>
+        <v>0.03153451873827431</v>
       </c>
       <c r="C12">
-        <v>0.005925969150221014</v>
+        <v>0.0001224608558743923</v>
       </c>
       <c r="D12">
-        <v>-16.69044967911166</v>
+        <v>257.5069275248179</v>
       </c>
       <c r="E12">
-        <v>1.538079251773006E-62</v>
+        <v>0</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="I12">
-        <v>0.9058268645769928</v>
+        <v>1.032036999595873</v>
       </c>
       <c r="J12">
-        <v>0.8953666413654091</v>
+        <v>1.031789316418768</v>
       </c>
       <c r="K12">
-        <v>0.9164092905428241</v>
+        <v>1.032284742229842</v>
       </c>
     </row>
     <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>sexMale</t>
+        </is>
+      </c>
       <c r="B13">
-        <v>-0.004082061512190049</v>
+        <v>0.1101025714176286</v>
       </c>
       <c r="C13">
-        <v>0.0001652141970043297</v>
+        <v>0.004097767859318931</v>
       </c>
       <c r="D13">
-        <v>-24.70769211245854</v>
+        <v>26.86891380809653</v>
       </c>
       <c r="E13">
-        <v>8.841224591584856E-135</v>
+        <v>3.653844870893365E-157</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="I13">
-        <v>0.9959262587757454</v>
+        <v>1.116392574555349</v>
       </c>
       <c r="J13">
-        <v>0.9956038103182112</v>
+        <v>1.107462039400485</v>
       </c>
       <c r="K13">
-        <v>0.9962488116653907</v>
+        <v>1.125395125233378</v>
       </c>
     </row>
     <row r="14">
@@ -787,195 +797,205 @@
         </is>
       </c>
       <c r="B14">
-        <v>-3.081931756694715</v>
+        <v>-2.88964647089247</v>
       </c>
       <c r="C14">
-        <v>0.01262510515580355</v>
+        <v>0.005781344367692456</v>
       </c>
       <c r="D14">
-        <v>-244.1113732251175</v>
+        <v>-499.8225822769718</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>fixed</t>
         </is>
       </c>
       <c r="I14">
-        <v>0.04587056024484683</v>
+        <v>0.05559586389377296</v>
       </c>
       <c r="J14">
-        <v>0.04474941250174443</v>
+        <v>0.05496943882822988</v>
       </c>
       <c r="K14">
-        <v>0.04701979712234433</v>
+        <v>0.0562294276234739</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>I(o_htn &gt;= 1)TRUE</t>
+          <t>I(o_htn_blood_related &gt;= 1)TRUE</t>
         </is>
       </c>
       <c r="B15">
-        <v>0.3730552400599209</v>
+        <v>0.1811974759670196</v>
       </c>
       <c r="C15">
-        <v>0.008148930703652036</v>
+        <v>0.003615188819240502</v>
       </c>
       <c r="D15">
-        <v>45.77965546973321</v>
+        <v>50.12116518027032</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>fixed</t>
         </is>
       </c>
       <c r="I15">
-        <v>1.45216455527425</v>
+        <v>1.198651860858313</v>
       </c>
       <c r="J15">
-        <v>1.429154964779104</v>
+        <v>1.190188509451303</v>
       </c>
       <c r="K15">
-        <v>1.475544603324946</v>
+        <v>1.207175394594819</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>blood_relation1</t>
+          <t>age</t>
         </is>
       </c>
       <c r="B16">
-        <v>0.2621065432250585</v>
+        <v>0.03097345953618993</v>
       </c>
       <c r="C16">
-        <v>0.01340743578699627</v>
+        <v>9.498626358678939E-05</v>
       </c>
       <c r="D16">
-        <v>19.5493416779421</v>
+        <v>326.0835658399105</v>
       </c>
       <c r="E16">
-        <v>1.402245588837192E-84</v>
+        <v>0</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>fixed</t>
         </is>
       </c>
       <c r="I16">
-        <v>1.299665005554284</v>
+        <v>1.03145812814612</v>
       </c>
       <c r="J16">
-        <v>1.265956507773555</v>
+        <v>1.031266116287262</v>
       </c>
       <c r="K16">
-        <v>1.334271056146391</v>
+        <v>1.031650175755745</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>age</t>
+          <t>sexMale</t>
         </is>
       </c>
       <c r="B17">
-        <v>0.0342949615130257</v>
+        <v>0.1158197485775821</v>
       </c>
       <c r="C17">
-        <v>0.0002283563519149615</v>
+        <v>0.003356411514289132</v>
       </c>
       <c r="D17">
-        <v>150.1817717152748</v>
+        <v>34.50701681975133</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>6.29535631061077E-261</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>fixed</t>
         </is>
       </c>
       <c r="I17">
-        <v>1.034889814379114</v>
+        <v>1.122793468772228</v>
       </c>
       <c r="J17">
-        <v>1.034426723642776</v>
+        <v>1.11543133987452</v>
       </c>
       <c r="K17">
-        <v>1.035353112431277</v>
+        <v>1.130204189582292</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>I(o_htn &gt;= 1)TRUE:blood_relation1</t>
+          <t>sd__(Intercept)</t>
         </is>
       </c>
       <c r="B18">
-        <v>-0.07794559820990996</v>
-      </c>
-      <c r="C18">
-        <v>0.006708189937668971</v>
-      </c>
-      <c r="D18">
-        <v>-11.61946798378748</v>
-      </c>
-      <c r="E18">
-        <v>3.825640744614236E-31</v>
+        <v>0</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>ran_pars</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>hhid:cluster</t>
         </is>
       </c>
       <c r="I18">
-        <v>0.9250147476328792</v>
-      </c>
-      <c r="J18">
-        <v>0.9129322103489704</v>
-      </c>
-      <c r="K18">
-        <v>0.9372571957026733</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>blood_relation1:age</t>
+          <t>sd__(Intercept)</t>
         </is>
       </c>
       <c r="B19">
-        <v>-0.004431394922940958</v>
-      </c>
-      <c r="C19">
-        <v>0.0002492484869192287</v>
-      </c>
-      <c r="D19">
-        <v>-17.77902436927127</v>
-      </c>
-      <c r="E19">
-        <v>2.357079438631633E-70</v>
+        <v>0.3329827193331942</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>ran_pars</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>cluster</t>
         </is>
       </c>
       <c r="I19">
-        <v>0.9955784092201841</v>
-      </c>
-      <c r="J19">
-        <v>0.9950921610348159</v>
-      </c>
-      <c r="K19">
-        <v>0.9960648950089696</v>
+        <v>1.395123189602503</v>
       </c>
     </row>
     <row r="20">
@@ -985,451 +1005,129 @@
         </is>
       </c>
       <c r="B20">
-        <v>-3.051075013741826</v>
+        <v>-2.822209626495849</v>
       </c>
       <c r="C20">
-        <v>0.009185424026358713</v>
+        <v>0.006090937535057383</v>
       </c>
       <c r="D20">
-        <v>-332.1648521599425</v>
+        <v>214689.2241158239</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>fixed</t>
+          <t>E</t>
         </is>
       </c>
       <c r="I20">
-        <v>0.04730804025209706</v>
+        <v>0.0594743812429986</v>
       </c>
       <c r="J20">
-        <v>0.04646395423048821</v>
+        <v>0.05876858332467561</v>
       </c>
       <c r="K20">
-        <v>0.04816746033693138</v>
+        <v>0.06018865564098688</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>I(o_htn &gt;= 1)TRUE</t>
+          <t>I(o_htn_blood_related &gt;= 1)TRUE</t>
         </is>
       </c>
       <c r="B21">
-        <v>0.4106034995152687</v>
+        <v>0.09594391468545097</v>
       </c>
       <c r="C21">
-        <v>0.005674695459882314</v>
+        <v>0.005096381457183439</v>
       </c>
       <c r="D21">
-        <v>72.35692248475024</v>
+        <v>354.4141193276413</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>fixed</t>
+          <t>E</t>
         </is>
       </c>
       <c r="I21">
-        <v>1.507727423371283</v>
+        <v>1.100697329306853</v>
       </c>
       <c r="J21">
-        <v>1.491050785266149</v>
+        <v>1.089757295784076</v>
       </c>
       <c r="K21">
-        <v>1.524590581118294</v>
+        <v>1.111747189424912</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>blood_relation1</t>
+          <t>age</t>
         </is>
       </c>
       <c r="B22">
-        <v>0.2641053348046307</v>
+        <v>0.03154712520904304</v>
       </c>
       <c r="C22">
-        <v>0.01103151540299746</v>
+        <v>9.803998211088932E-05</v>
       </c>
       <c r="D22">
-        <v>23.94098409479341</v>
+        <v>103541.1852964881</v>
       </c>
       <c r="E22">
-        <v>1.147105380966455E-126</v>
+        <v>0</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>fixed</t>
+          <t>E</t>
         </is>
       </c>
       <c r="I22">
-        <v>1.30226536294414</v>
+        <v>1.032050010022148</v>
       </c>
       <c r="J22">
-        <v>1.274410303566995</v>
+        <v>1.031851712032608</v>
       </c>
       <c r="K22">
-        <v>1.330729256329242</v>
+        <v>1.032248346119968</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>age</t>
+          <t>sexMale</t>
         </is>
       </c>
       <c r="B23">
-        <v>0.03334374948203384</v>
+        <v>0.0802801288535519</v>
       </c>
       <c r="C23">
-        <v>0.000183288579914991</v>
+        <v>0.003754732248692577</v>
       </c>
       <c r="D23">
-        <v>181.9194054397641</v>
+        <v>457.1494233280751</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>fixed</t>
+          <t>E</t>
         </is>
       </c>
       <c r="I23">
-        <v>1.033905882774904</v>
+        <v>1.083590570147209</v>
       </c>
       <c r="J23">
-        <v>1.033534523327127</v>
+        <v>1.075645400134121</v>
       </c>
       <c r="K23">
-        <v>1.034277375655902</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>I(o_htn &gt;= 1)TRUE:blood_relation1</t>
-        </is>
-      </c>
-      <c r="B24">
-        <v>-0.09890656793262931</v>
-      </c>
-      <c r="C24">
-        <v>0.006991656741802281</v>
-      </c>
-      <c r="D24">
-        <v>-14.14637067939545</v>
-      </c>
-      <c r="E24">
-        <v>1.966473747133887E-45</v>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>fixed</t>
-        </is>
-      </c>
-      <c r="I24">
-        <v>0.9058273373907518</v>
-      </c>
-      <c r="J24">
-        <v>0.8934988645731701</v>
-      </c>
-      <c r="K24">
-        <v>0.9183259181380022</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>blood_relation1:age</t>
-        </is>
-      </c>
-      <c r="B25">
-        <v>-0.004081909425600072</v>
-      </c>
-      <c r="C25">
-        <v>0.0002123747507021117</v>
-      </c>
-      <c r="D25">
-        <v>-19.22031414801084</v>
-      </c>
-      <c r="E25">
-        <v>2.502503640105058E-82</v>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>fixed</t>
-        </is>
-      </c>
-      <c r="I25">
-        <v>0.9959264102427855</v>
-      </c>
-      <c r="J25">
-        <v>0.995511937650551</v>
-      </c>
-      <c r="K25">
-        <v>0.9963410553970187</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>sd__(Intercept)</t>
-        </is>
-      </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>ran_pars</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>cluster_hhid</t>
-        </is>
-      </c>
-      <c r="I26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>(Intercept)</t>
-        </is>
-      </c>
-      <c r="B27">
-        <v>-2.996374392703168</v>
-      </c>
-      <c r="C27">
-        <v>0.01057366399010294</v>
-      </c>
-      <c r="D27">
-        <v>80304.73313889312</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="I27">
-        <v>0.04996790434826024</v>
-      </c>
-      <c r="J27">
-        <v>0.04894300730093124</v>
-      </c>
-      <c r="K27">
-        <v>0.05101426337791421</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>I(o_htn &gt;= 1)TRUE</t>
-        </is>
-      </c>
-      <c r="B28">
-        <v>0.1462374268781028</v>
-      </c>
-      <c r="C28">
-        <v>0.007271317603498713</v>
-      </c>
-      <c r="D28">
-        <v>404.4742184233245</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="I28">
-        <v>1.157470970148115</v>
-      </c>
-      <c r="J28">
-        <v>1.141091938061981</v>
-      </c>
-      <c r="K28">
-        <v>1.174085103967185</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>blood_relation1</t>
-        </is>
-      </c>
-      <c r="B29">
-        <v>0.2819365589960387</v>
-      </c>
-      <c r="C29">
-        <v>0.01219729384359471</v>
-      </c>
-      <c r="D29">
-        <v>534.2884881094592</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="I29">
-        <v>1.32569461392168</v>
-      </c>
-      <c r="J29">
-        <v>1.294377472122548</v>
-      </c>
-      <c r="K29">
-        <v>1.357769466196767</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>age</t>
-        </is>
-      </c>
-      <c r="B30">
-        <v>0.03527641318121918</v>
-      </c>
-      <c r="C30">
-        <v>0.0002017401709534023</v>
-      </c>
-      <c r="D30">
-        <v>30576.23956342332</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="I30">
-        <v>1.035906007304383</v>
-      </c>
-      <c r="J30">
-        <v>1.035496479919671</v>
-      </c>
-      <c r="K30">
-        <v>1.036315696652639</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>I(o_htn &gt;= 1)TRUE:blood_relation1</t>
-        </is>
-      </c>
-      <c r="B31">
-        <v>-0.0635716326463597</v>
-      </c>
-      <c r="C31">
-        <v>0.00628303497452089</v>
-      </c>
-      <c r="D31">
-        <v>102.3735528882605</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="I31">
-        <v>0.938406896323667</v>
-      </c>
-      <c r="J31">
-        <v>0.926921516290379</v>
-      </c>
-      <c r="K31">
-        <v>0.9500345904064087</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>blood_relation1:age</t>
-        </is>
-      </c>
-      <c r="B32">
-        <v>-0.005215872923376849</v>
-      </c>
-      <c r="C32">
-        <v>0.0002305154015592078</v>
-      </c>
-      <c r="D32">
-        <v>511.9813120253262</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="I32">
-        <v>0.9947977061226818</v>
-      </c>
-      <c r="J32">
-        <v>0.9943483479049499</v>
-      </c>
-      <c r="K32">
-        <v>0.9952472674109054</v>
+        <v>1.091594426532711</v>
       </c>
     </row>
   </sheetData>

</xml_diff>